<commit_message>
cosas para añadir al ppt
</commit_message>
<xml_diff>
--- a/datos/imagenes/Arturo/video-6/video-6.xlsx
+++ b/datos/imagenes/Arturo/video-6/video-6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\notebooks\Paper interferometria\Interferometria - GUA\datos\imagenes\Arturo\video-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D8B83-D022-4FF8-BD31-AF2F2EBB9A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432963E-5EC4-48B7-A2DF-B6DDC28128AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10812" yWindow="-300" windowWidth="12072" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +130,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +159,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -225,15 +237,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5"/>
@@ -248,9 +261,11 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="6" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Énfasis1" xfId="5" builtinId="30"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26"/>
     <cellStyle name="Cálculo" xfId="4" builtinId="22"/>
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +559,7 @@
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -584,35 +599,35 @@
         <v>1</v>
       </c>
       <c r="C2" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="9">
-        <v>245.2</v>
+        <v>253.5</v>
       </c>
       <c r="E2" s="9">
-        <v>109.7</v>
+        <v>106.7</v>
       </c>
       <c r="F2" s="9">
-        <v>122.1</v>
+        <v>100.5</v>
       </c>
       <c r="G2" s="4">
         <f>(E2+F2)/2</f>
-        <v>115.9</v>
+        <v>103.6</v>
       </c>
       <c r="H2" s="5">
         <f>(D2-G2)/(D2+G2)</f>
-        <v>0.35807255607864852</v>
+        <v>0.41977037244469334</v>
       </c>
       <c r="I2" s="6">
         <f>AVERAGE(H2:H11)</f>
-        <v>0.34416740972202953</v>
+        <v>0.45772079833774859</v>
       </c>
       <c r="J2" s="6">
         <f>STDEVA(H2:H11)</f>
-        <v>6.5484623693708596E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.4449521834762375E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -620,29 +635,32 @@
         <v>2</v>
       </c>
       <c r="C3" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" s="9">
-        <v>252.3</v>
+        <v>250</v>
       </c>
       <c r="E3" s="9">
-        <v>110.8</v>
+        <v>98</v>
       </c>
       <c r="F3" s="9">
-        <v>120.1</v>
+        <v>101.3</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" ref="G3:G11" si="0">(E3+F3)/2</f>
-        <v>115.44999999999999</v>
+        <v>99.65</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H11" si="1">(D3-G3)/(D3+G3)</f>
-        <v>0.37212780421481989</v>
+        <v>0.43000143000143004</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -650,29 +668,29 @@
         <v>3</v>
       </c>
       <c r="C4" s="8">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9">
-        <v>189.6</v>
+        <v>248.8</v>
       </c>
       <c r="E4" s="9">
-        <v>143.6</v>
+        <v>121.5</v>
       </c>
       <c r="F4" s="9">
-        <v>96.7</v>
+        <v>121.8</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>120.15</v>
+        <v>121.65</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="1"/>
-        <v>0.22421307506053265</v>
+        <v>0.34323120529086243</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -680,29 +698,29 @@
         <v>4</v>
       </c>
       <c r="C5" s="11">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D5" s="9">
-        <v>240.9</v>
+        <v>251.5</v>
       </c>
       <c r="E5" s="9">
-        <v>127.6</v>
+        <v>116.8</v>
       </c>
       <c r="F5" s="9">
-        <v>97.4</v>
+        <v>102.6</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>112.5</v>
+        <v>109.69999999999999</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="1"/>
-        <v>0.36332767402376914</v>
+        <v>0.39258028792912519</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -710,29 +728,29 @@
         <v>5</v>
       </c>
       <c r="C6" s="11">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D6" s="9">
-        <v>248</v>
+        <v>248.8</v>
       </c>
       <c r="E6" s="9">
-        <v>121.3</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="F6" s="9">
-        <v>121.7</v>
+        <v>73.7</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>121.5</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>0.34235453315290931</v>
+        <v>0.52825552825552824</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -740,59 +758,59 @@
         <v>6</v>
       </c>
       <c r="C7" s="11">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
-        <v>247.1</v>
+        <v>240.7</v>
       </c>
       <c r="E7" s="9">
-        <v>93.4</v>
+        <v>100.4</v>
       </c>
       <c r="F7" s="9">
-        <v>103.5</v>
+        <v>102.1</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>98.45</v>
+        <v>101.25</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
-        <v>0.43018376501229916</v>
+        <v>0.40780815908758589</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
-        <v>90</v>
+      <c r="C8" s="12">
+        <v>66</v>
       </c>
       <c r="D8" s="9">
-        <v>175.3</v>
+        <v>252.2</v>
       </c>
       <c r="E8" s="9">
-        <v>121.3</v>
+        <v>70.3</v>
       </c>
       <c r="F8" s="9">
-        <v>79</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>100.15</v>
+        <v>67.849999999999994</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="1"/>
-        <v>0.27282628426211653</v>
+        <v>0.57600374941415411</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -800,29 +818,29 @@
         <v>8</v>
       </c>
       <c r="C9" s="11">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D9" s="9">
-        <v>236.8</v>
+        <v>250.4</v>
       </c>
       <c r="E9" s="9">
-        <v>158.4</v>
+        <v>85.8</v>
       </c>
       <c r="F9" s="9">
-        <v>104.9</v>
+        <v>83</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>131.65</v>
+        <v>84.4</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
-        <v>0.2853847197720179</v>
+        <v>0.49581839904420549</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -830,29 +848,29 @@
         <v>9</v>
       </c>
       <c r="C10" s="11">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="D10" s="9">
         <v>251.2</v>
       </c>
       <c r="E10" s="9">
-        <v>96.5</v>
+        <v>76</v>
       </c>
       <c r="F10" s="9">
-        <v>107.1</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>101.8</v>
+        <v>74.55</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
-        <v>0.42322946175637388</v>
+        <v>0.54228702993092859</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -860,24 +878,24 @@
         <v>10</v>
       </c>
       <c r="C11" s="11">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D11" s="10">
-        <v>246.9</v>
+        <v>250.2</v>
       </c>
       <c r="E11" s="10">
-        <v>105.1</v>
+        <v>93.9</v>
       </c>
       <c r="F11" s="10">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>113.55</v>
+        <v>96.95</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="1"/>
-        <v>0.36995422388680821</v>
+        <v>0.44145182197897165</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>

</xml_diff>